<commit_message>
Fixed bug getting date
</commit_message>
<xml_diff>
--- a/outputs/Table.xlsx
+++ b/outputs/Table.xlsx
@@ -436,12 +436,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sat Oct 24 23:45:09 2020</t>
+          <t>2020/07/25 02:22:07</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Test.txt</t>
+          <t>WhatsApp Image 2020-10-25 at 1.23.13 AM.jpeg</t>
         </is>
       </c>
     </row>

</xml_diff>